<commit_message>
add paa on  all pages
</commit_message>
<xml_diff>
--- a/VAS-SHEET.xlsx
+++ b/VAS-SHEET.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://olxlb-my.sharepoint.com/personal/ranime_merhi_olxlb_onmicrosoft_com/Documents/Desktop/Product-v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{4651F941-BBE8-442D-B8CE-B6F4C6BB6DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3553C2BF-6119-4CC0-86B8-992647FDAC3D}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{4651F941-BBE8-442D-B8CE-B6F4C6BB6DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAF67C3B-BCEC-4B32-B852-AFE5A3F9BCE1}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7B2C9A5A-8472-4594-B453-3A71EB36BA2F}"/>
   </bookViews>
@@ -877,6 +877,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1194,13 +1198,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5FDCEE0-F19C-462F-9C6A-117F5A0AAFD7}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:X586"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:V1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1332,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1447,7 +1455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1562,7 +1570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1692,7 +1700,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1875,7 +1883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -2102,7 +2110,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2173,7 +2181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -2232,7 +2240,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -2291,7 +2299,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2350,7 +2358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2409,7 +2417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -2471,7 +2479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2533,7 +2541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -2595,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -2651,7 +2659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -2719,7 +2727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -2778,7 +2786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -2837,7 +2845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -2899,7 +2907,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -2961,7 +2969,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -3023,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -3082,7 +3090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -3141,7 +3149,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -3200,7 +3208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -3371,7 +3379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>48</v>
       </c>
@@ -3445,7 +3453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3504,7 +3512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>24</v>
       </c>
@@ -3563,7 +3571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -3622,7 +3630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>24</v>
       </c>
@@ -3681,7 +3689,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -3858,7 +3866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
@@ -3932,7 +3940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -3991,7 +3999,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>24</v>
       </c>
@@ -4056,7 +4064,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -4124,7 +4132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -4186,7 +4194,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -4248,7 +4256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -4310,7 +4318,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -4369,7 +4377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -4431,7 +4439,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -4499,7 +4507,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>48</v>
       </c>
@@ -4564,7 +4572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -4626,7 +4634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>48</v>
       </c>
@@ -4685,7 +4693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>48</v>
       </c>
@@ -4747,7 +4755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -4806,7 +4814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>48</v>
       </c>
@@ -4874,7 +4882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>48</v>
       </c>
@@ -4936,7 +4944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>48</v>
       </c>
@@ -4998,7 +5006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>146</v>
       </c>
@@ -5054,7 +5062,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>146</v>
       </c>
@@ -5119,7 +5127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>146</v>
       </c>
@@ -5184,7 +5192,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>146</v>
       </c>
@@ -5243,7 +5251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>146</v>
       </c>
@@ -5299,7 +5307,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>146</v>
       </c>
@@ -5358,7 +5366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>146</v>
       </c>
@@ -5414,7 +5422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>146</v>
       </c>
@@ -5473,7 +5481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>146</v>
       </c>
@@ -5529,7 +5537,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>146</v>
       </c>
@@ -5585,7 +5593,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>146</v>
       </c>
@@ -5641,7 +5649,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>146</v>
       </c>
@@ -5703,7 +5711,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -5768,7 +5776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>146</v>
       </c>
@@ -5827,7 +5835,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>146</v>
       </c>
@@ -5886,7 +5894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>146</v>
       </c>
@@ -5942,7 +5950,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>146</v>
       </c>
@@ -6001,7 +6009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>146</v>
       </c>
@@ -6057,7 +6065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>146</v>
       </c>
@@ -6113,7 +6121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>146</v>
       </c>
@@ -6169,7 +6177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>146</v>
       </c>
@@ -6228,7 +6236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>146</v>
       </c>
@@ -6284,7 +6292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>146</v>
       </c>
@@ -6346,7 +6354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>146</v>
       </c>
@@ -6402,7 +6410,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>146</v>
       </c>
@@ -6467,7 +6475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>146</v>
       </c>
@@ -6532,7 +6540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>146</v>
       </c>
@@ -6597,7 +6605,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>146</v>
       </c>
@@ -6662,7 +6670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>146</v>
       </c>
@@ -6718,7 +6726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>146</v>
       </c>
@@ -6774,7 +6782,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>146</v>
       </c>
@@ -6830,7 +6838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>146</v>
       </c>
@@ -6889,7 +6897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>48</v>
       </c>
@@ -6951,7 +6959,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -7013,7 +7021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>48</v>
       </c>
@@ -7075,7 +7083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>48</v>
       </c>
@@ -7134,7 +7142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>48</v>
       </c>
@@ -7193,7 +7201,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>48</v>
       </c>
@@ -7261,7 +7269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -7329,7 +7337,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -7385,7 +7393,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>48</v>
       </c>
@@ -7447,7 +7455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -7509,7 +7517,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>48</v>
       </c>
@@ -7571,7 +7579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>48</v>
       </c>
@@ -7633,7 +7641,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>48</v>
       </c>
@@ -7692,7 +7700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>48</v>
       </c>
@@ -7754,7 +7762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>48</v>
       </c>
@@ -7813,7 +7821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>48</v>
       </c>
@@ -7875,7 +7883,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>48</v>
       </c>
@@ -7934,7 +7942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>48</v>
       </c>
@@ -7996,7 +8004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>48</v>
       </c>
@@ -8058,7 +8066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>48</v>
       </c>
@@ -8117,7 +8125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>48</v>
       </c>
@@ -8176,7 +8184,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>48</v>
       </c>
@@ -8235,7 +8243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>48</v>
       </c>
@@ -8297,7 +8305,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -8359,7 +8367,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>48</v>
       </c>
@@ -8421,7 +8429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>48</v>
       </c>
@@ -8483,7 +8491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>48</v>
       </c>
@@ -8542,7 +8550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>146</v>
       </c>
@@ -8598,7 +8606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>146</v>
       </c>
@@ -8654,7 +8662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>146</v>
       </c>
@@ -8713,7 +8721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>146</v>
       </c>
@@ -8778,7 +8786,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>146</v>
       </c>
@@ -8834,7 +8842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>146</v>
       </c>
@@ -8905,7 +8913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>146</v>
       </c>
@@ -8961,7 +8969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>146</v>
       </c>
@@ -9029,7 +9037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>146</v>
       </c>
@@ -9088,7 +9096,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>146</v>
       </c>
@@ -9144,7 +9152,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>146</v>
       </c>
@@ -9200,7 +9208,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>146</v>
       </c>
@@ -9268,7 +9276,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>146</v>
       </c>
@@ -9327,7 +9335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>146</v>
       </c>
@@ -9398,7 +9406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>146</v>
       </c>
@@ -9457,7 +9465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>146</v>
       </c>
@@ -9516,7 +9524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>146</v>
       </c>
@@ -9572,7 +9580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>146</v>
       </c>
@@ -9634,7 +9642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>146</v>
       </c>
@@ -9693,7 +9701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>146</v>
       </c>
@@ -9749,7 +9757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>146</v>
       </c>
@@ -9808,7 +9816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>146</v>
       </c>
@@ -9873,7 +9881,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>146</v>
       </c>
@@ -9932,7 +9940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>146</v>
       </c>
@@ -10003,7 +10011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>146</v>
       </c>
@@ -10068,7 +10076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -10133,7 +10141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>146</v>
       </c>
@@ -10198,7 +10206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>146</v>
       </c>
@@ -10254,7 +10262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>146</v>
       </c>
@@ -10310,7 +10318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>146</v>
       </c>
@@ -10381,7 +10389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>146</v>
       </c>
@@ -10440,7 +10448,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>146</v>
       </c>
@@ -10511,7 +10519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>146</v>
       </c>
@@ -10573,7 +10581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>146</v>
       </c>
@@ -10638,7 +10646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>146</v>
       </c>
@@ -10703,7 +10711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>146</v>
       </c>
@@ -10762,7 +10770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>146</v>
       </c>
@@ -10821,7 +10829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>146</v>
       </c>
@@ -10886,7 +10894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>146</v>
       </c>
@@ -10942,7 +10950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>146</v>
       </c>
@@ -11001,7 +11009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>146</v>
       </c>
@@ -11060,7 +11068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>146</v>
       </c>
@@ -11116,7 +11124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>146</v>
       </c>
@@ -11181,7 +11189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>146</v>
       </c>
@@ -11246,7 +11254,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>146</v>
       </c>
@@ -11308,7 +11316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>146</v>
       </c>
@@ -11373,7 +11381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>48</v>
       </c>
@@ -11435,7 +11443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>48</v>
       </c>
@@ -11494,7 +11502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>48</v>
       </c>
@@ -11556,7 +11564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>48</v>
       </c>
@@ -11615,7 +11623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>48</v>
       </c>
@@ -11674,7 +11682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>48</v>
       </c>
@@ -11733,7 +11741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>48</v>
       </c>
@@ -11792,7 +11800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>48</v>
       </c>
@@ -11854,7 +11862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>48</v>
       </c>
@@ -11916,7 +11924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>48</v>
       </c>
@@ -11978,7 +11986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -12040,7 +12048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>48</v>
       </c>
@@ -12099,7 +12107,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>48</v>
       </c>
@@ -12167,7 +12175,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>48</v>
       </c>
@@ -12229,7 +12237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>48</v>
       </c>
@@ -12297,7 +12305,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>48</v>
       </c>
@@ -12365,7 +12373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>48</v>
       </c>
@@ -12430,7 +12438,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>48</v>
       </c>
@@ -12498,7 +12506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>48</v>
       </c>
@@ -12566,7 +12574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>48</v>
       </c>
@@ -12634,7 +12642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>48</v>
       </c>
@@ -12708,7 +12716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>48</v>
       </c>
@@ -12773,7 +12781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>48</v>
       </c>
@@ -12841,7 +12849,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>48</v>
       </c>
@@ -12909,7 +12917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>48</v>
       </c>
@@ -12974,7 +12982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>48</v>
       </c>
@@ -13042,7 +13050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>48</v>
       </c>
@@ -13110,7 +13118,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>48</v>
       </c>
@@ -13178,7 +13186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>48</v>
       </c>
@@ -13246,7 +13254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>48</v>
       </c>
@@ -13432,7 +13440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>24</v>
       </c>
@@ -13544,7 +13552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>48</v>
       </c>
@@ -13618,7 +13626,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>24</v>
       </c>
@@ -13677,7 +13685,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>24</v>
       </c>
@@ -13798,7 +13806,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>24</v>
       </c>
@@ -13857,7 +13865,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>48</v>
       </c>
@@ -13984,7 +13992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>48</v>
       </c>
@@ -14058,7 +14066,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>24</v>
       </c>
@@ -14173,7 +14181,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>48</v>
       </c>
@@ -14235,7 +14243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>48</v>
       </c>
@@ -14294,7 +14302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>48</v>
       </c>
@@ -14353,7 +14361,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>48</v>
       </c>
@@ -14415,7 +14423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>48</v>
       </c>
@@ -14477,7 +14485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>48</v>
       </c>
@@ -14539,7 +14547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>48</v>
       </c>
@@ -14598,7 +14606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>48</v>
       </c>
@@ -14660,7 +14668,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>48</v>
       </c>
@@ -14719,7 +14727,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>48</v>
       </c>
@@ -14781,7 +14789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>48</v>
       </c>
@@ -14843,7 +14851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>48</v>
       </c>
@@ -14905,7 +14913,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>48</v>
       </c>
@@ -14967,7 +14975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>48</v>
       </c>
@@ -15029,7 +15037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>48</v>
       </c>
@@ -15088,7 +15096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="227" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>48</v>
       </c>
@@ -15147,7 +15155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>48</v>
       </c>
@@ -15209,7 +15217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>48</v>
       </c>
@@ -15277,7 +15285,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>24</v>
       </c>
@@ -15336,7 +15344,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>48</v>
       </c>
@@ -15401,7 +15409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>48</v>
       </c>
@@ -15469,7 +15477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>48</v>
       </c>
@@ -15537,7 +15545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>48</v>
       </c>
@@ -15605,7 +15613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>24</v>
       </c>
@@ -15664,7 +15672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="236" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>48</v>
       </c>
@@ -15732,7 +15740,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>48</v>
       </c>
@@ -15800,7 +15808,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>48</v>
       </c>
@@ -15865,7 +15873,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>48</v>
       </c>
@@ -15933,7 +15941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>24</v>
       </c>
@@ -15992,7 +16000,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>48</v>
       </c>
@@ -16060,7 +16068,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>48</v>
       </c>
@@ -16128,7 +16136,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>146</v>
       </c>
@@ -16193,7 +16201,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>146</v>
       </c>
@@ -16258,7 +16266,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>146</v>
       </c>
@@ -16323,7 +16331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>146</v>
       </c>
@@ -16388,7 +16396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>146</v>
       </c>
@@ -16453,7 +16461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>146</v>
       </c>
@@ -16512,7 +16520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>146</v>
       </c>
@@ -16568,7 +16576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>146</v>
       </c>
@@ -16624,7 +16632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>146</v>
       </c>
@@ -16686,7 +16694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>146</v>
       </c>
@@ -16742,7 +16750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>146</v>
       </c>
@@ -16807,7 +16815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>146</v>
       </c>
@@ -16863,7 +16871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>146</v>
       </c>
@@ -16919,7 +16927,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>146</v>
       </c>
@@ -16984,7 +16992,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>146</v>
       </c>
@@ -17043,7 +17051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>48</v>
       </c>
@@ -17105,7 +17113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>24</v>
       </c>
@@ -17170,7 +17178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>24</v>
       </c>
@@ -17229,7 +17237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>48</v>
       </c>
@@ -17291,7 +17299,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>48</v>
       </c>
@@ -17353,7 +17361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>48</v>
       </c>
@@ -17415,7 +17423,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>48</v>
       </c>
@@ -17471,7 +17479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>48</v>
       </c>
@@ -17530,7 +17538,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>48</v>
       </c>
@@ -17592,7 +17600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>24</v>
       </c>
@@ -17651,7 +17659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>48</v>
       </c>
@@ -17713,7 +17721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>48</v>
       </c>
@@ -17772,7 +17780,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>24</v>
       </c>
@@ -17837,7 +17845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>24</v>
       </c>
@@ -17896,7 +17904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>48</v>
       </c>
@@ -17958,7 +17966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>48</v>
       </c>
@@ -18017,7 +18025,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>48</v>
       </c>
@@ -18076,7 +18084,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>48</v>
       </c>
@@ -18138,7 +18146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>48</v>
       </c>
@@ -18197,7 +18205,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>48</v>
       </c>
@@ -18256,7 +18264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>48</v>
       </c>
@@ -18318,7 +18326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>48</v>
       </c>
@@ -18380,7 +18388,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>48</v>
       </c>
@@ -18442,7 +18450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>48</v>
       </c>
@@ -18501,7 +18509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>48</v>
       </c>
@@ -18569,7 +18577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>48</v>
       </c>
@@ -18631,7 +18639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>48</v>
       </c>
@@ -18693,7 +18701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>48</v>
       </c>
@@ -18755,7 +18763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>48</v>
       </c>
@@ -18817,7 +18825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>48</v>
       </c>
@@ -18879,7 +18887,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>48</v>
       </c>
@@ -19009,7 +19017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>48</v>
       </c>
@@ -19245,7 +19253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>24</v>
       </c>
@@ -19304,7 +19312,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="295" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>48</v>
       </c>
@@ -19434,7 +19442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>48</v>
       </c>
@@ -19499,7 +19507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="298" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>24</v>
       </c>
@@ -19558,7 +19566,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="299" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>24</v>
       </c>
@@ -19617,7 +19625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="300" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>24</v>
       </c>
@@ -19794,7 +19802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>48</v>
       </c>
@@ -19856,7 +19864,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="304" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>146</v>
       </c>
@@ -19915,7 +19923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>146</v>
       </c>
@@ -19986,7 +19994,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="306" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>146</v>
       </c>
@@ -20042,7 +20050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="307" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>146</v>
       </c>
@@ -20107,7 +20115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="308" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>146</v>
       </c>
@@ -20163,7 +20171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="309" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>146</v>
       </c>
@@ -20222,7 +20230,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="310" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>146</v>
       </c>
@@ -20290,7 +20298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="311" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>146</v>
       </c>
@@ -20349,7 +20357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="312" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>146</v>
       </c>
@@ -20408,7 +20416,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="313" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>146</v>
       </c>
@@ -20479,7 +20487,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="314" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>146</v>
       </c>
@@ -20538,7 +20546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="315" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>146</v>
       </c>
@@ -20609,7 +20617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>146</v>
       </c>
@@ -20665,7 +20673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="317" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>146</v>
       </c>
@@ -20727,7 +20735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>146</v>
       </c>
@@ -20792,7 +20800,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="319" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>24</v>
       </c>
@@ -21075,7 +21083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="324" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>48</v>
       </c>
@@ -21314,7 +21322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="328" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>48</v>
       </c>
@@ -21379,7 +21387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="329" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>24</v>
       </c>
@@ -21438,7 +21446,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>48</v>
       </c>
@@ -21509,7 +21517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>48</v>
       </c>
@@ -21580,7 +21588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>24</v>
       </c>
@@ -21751,7 +21759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="335" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>48</v>
       </c>
@@ -21825,7 +21833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>146</v>
       </c>
@@ -21881,7 +21889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="337" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>146</v>
       </c>
@@ -21946,7 +21954,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="338" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>146</v>
       </c>
@@ -22011,7 +22019,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="339" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>146</v>
       </c>
@@ -22073,7 +22081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="340" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>146</v>
       </c>
@@ -22132,7 +22140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="341" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>146</v>
       </c>
@@ -22197,7 +22205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="342" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>146</v>
       </c>
@@ -22262,7 +22270,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="343" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>146</v>
       </c>
@@ -22321,7 +22329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>146</v>
       </c>
@@ -22380,7 +22388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>146</v>
       </c>
@@ -22436,7 +22444,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="346" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>146</v>
       </c>
@@ -22501,7 +22509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="347" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>146</v>
       </c>
@@ -22566,7 +22574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="348" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>146</v>
       </c>
@@ -22619,7 +22627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="349" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>146</v>
       </c>
@@ -22675,7 +22683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="350" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>146</v>
       </c>
@@ -22740,7 +22748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="351" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>146</v>
       </c>
@@ -22799,7 +22807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>146</v>
       </c>
@@ -22861,7 +22869,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="353" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>146</v>
       </c>
@@ -22917,7 +22925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="354" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>146</v>
       </c>
@@ -22973,7 +22981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="355" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>146</v>
       </c>
@@ -23044,7 +23052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>146</v>
       </c>
@@ -23103,7 +23111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>146</v>
       </c>
@@ -23162,7 +23170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>146</v>
       </c>
@@ -23218,7 +23226,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="359" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>146</v>
       </c>
@@ -23280,7 +23288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="360" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>146</v>
       </c>
@@ -23339,7 +23347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="361" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>146</v>
       </c>
@@ -23404,7 +23412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="362" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>146</v>
       </c>
@@ -23463,7 +23471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>146</v>
       </c>
@@ -23522,7 +23530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="364" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>146</v>
       </c>
@@ -23578,7 +23586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="365" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>146</v>
       </c>
@@ -23646,7 +23654,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="366" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>146</v>
       </c>
@@ -23702,7 +23710,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="367" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>146</v>
       </c>
@@ -23761,7 +23769,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="368" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>146</v>
       </c>
@@ -23826,7 +23834,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="369" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>146</v>
       </c>
@@ -23891,7 +23899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>146</v>
       </c>
@@ -23950,7 +23958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>146</v>
       </c>
@@ -24012,7 +24020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="372" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>146</v>
       </c>
@@ -24071,7 +24079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="373" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>146</v>
       </c>
@@ -24130,7 +24138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="374" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>146</v>
       </c>
@@ -24192,7 +24200,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="375" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>146</v>
       </c>
@@ -24257,7 +24265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="376" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>146</v>
       </c>
@@ -24319,7 +24327,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="377" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>146</v>
       </c>
@@ -24375,7 +24383,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="378" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>146</v>
       </c>
@@ -24437,7 +24445,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="379" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>146</v>
       </c>
@@ -24502,7 +24510,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="380" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>146</v>
       </c>
@@ -24561,7 +24569,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="381" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>146</v>
       </c>
@@ -24620,7 +24628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>48</v>
       </c>
@@ -24688,7 +24696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="383" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>48</v>
       </c>
@@ -24756,7 +24764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>48</v>
       </c>
@@ -24824,7 +24832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>48</v>
       </c>
@@ -24889,7 +24897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="386" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>48</v>
       </c>
@@ -24957,7 +24965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="387" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>48</v>
       </c>
@@ -25025,7 +25033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="388" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>48</v>
       </c>
@@ -25093,7 +25101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="389" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>48</v>
       </c>
@@ -25161,7 +25169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>48</v>
       </c>
@@ -25226,7 +25234,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="391" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>48</v>
       </c>
@@ -25291,7 +25299,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="392" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>48</v>
       </c>
@@ -25359,7 +25367,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="393" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>48</v>
       </c>
@@ -25424,7 +25432,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="394" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>48</v>
       </c>
@@ -25489,7 +25497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="395" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>48</v>
       </c>
@@ -25557,7 +25565,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="396" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>48</v>
       </c>
@@ -25616,7 +25624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="397" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>48</v>
       </c>
@@ -25684,7 +25692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="398" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>48</v>
       </c>
@@ -25746,7 +25754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="399" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>48</v>
       </c>
@@ -25805,7 +25813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="400" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>48</v>
       </c>
@@ -25867,7 +25875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="401" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>48</v>
       </c>
@@ -25929,7 +25937,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="402" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>48</v>
       </c>
@@ -25988,7 +25996,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="403" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>48</v>
       </c>
@@ -26047,7 +26055,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="404" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>48</v>
       </c>
@@ -26109,7 +26117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="405" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>48</v>
       </c>
@@ -26171,7 +26179,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="406" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>48</v>
       </c>
@@ -26233,7 +26241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="407" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>48</v>
       </c>
@@ -26295,7 +26303,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="408" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>48</v>
       </c>
@@ -26351,7 +26359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="409" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>146</v>
       </c>
@@ -26416,7 +26424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>146</v>
       </c>
@@ -26478,7 +26486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="411" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>146</v>
       </c>
@@ -26543,7 +26551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="412" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>146</v>
       </c>
@@ -26608,7 +26616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="413" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>146</v>
       </c>
@@ -26664,7 +26672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="414" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>146</v>
       </c>
@@ -26720,7 +26728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="415" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>146</v>
       </c>
@@ -26776,7 +26784,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="416" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>146</v>
       </c>
@@ -26832,7 +26840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="417" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>146</v>
       </c>
@@ -26897,7 +26905,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="418" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>146</v>
       </c>
@@ -26962,7 +26970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>146</v>
       </c>
@@ -27021,7 +27029,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="420" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>146</v>
       </c>
@@ -27083,7 +27091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="421" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>146</v>
       </c>
@@ -27148,7 +27156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="422" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>146</v>
       </c>
@@ -27204,7 +27212,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="423" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>146</v>
       </c>
@@ -27260,7 +27268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="424" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>146</v>
       </c>
@@ -27316,7 +27324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="425" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>48</v>
       </c>
@@ -27378,7 +27386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="426" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>48</v>
       </c>
@@ -27440,7 +27448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>48</v>
       </c>
@@ -27499,7 +27507,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="428" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>48</v>
       </c>
@@ -27567,7 +27575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="429" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>48</v>
       </c>
@@ -27626,7 +27634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="430" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>48</v>
       </c>
@@ -27688,7 +27696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>48</v>
       </c>
@@ -27750,7 +27758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>48</v>
       </c>
@@ -27809,7 +27817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="433" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>48</v>
       </c>
@@ -27871,7 +27879,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="434" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>48</v>
       </c>
@@ -27939,7 +27947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="435" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>48</v>
       </c>
@@ -28001,7 +28009,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="436" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>48</v>
       </c>
@@ -28060,7 +28068,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="437" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>48</v>
       </c>
@@ -28119,7 +28127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="438" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>48</v>
       </c>
@@ -28187,7 +28195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="439" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>48</v>
       </c>
@@ -28246,7 +28254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="440" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>146</v>
       </c>
@@ -28305,7 +28313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="441" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>146</v>
       </c>
@@ -28364,7 +28372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="442" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>146</v>
       </c>
@@ -28426,7 +28434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="443" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>146</v>
       </c>
@@ -28485,7 +28493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="444" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>146</v>
       </c>
@@ -28553,7 +28561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="445" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>146</v>
       </c>
@@ -28621,7 +28629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="446" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>146</v>
       </c>
@@ -28680,7 +28688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="447" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>146</v>
       </c>
@@ -28751,7 +28759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="448" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>146</v>
       </c>
@@ -28807,7 +28815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="449" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>146</v>
       </c>
@@ -28869,7 +28877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="450" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>146</v>
       </c>
@@ -28931,7 +28939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="451" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>146</v>
       </c>
@@ -28999,7 +29007,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="452" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>146</v>
       </c>
@@ -29055,7 +29063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="453" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>146</v>
       </c>
@@ -29114,7 +29122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="454" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>146</v>
       </c>
@@ -29182,7 +29190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="455" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>24</v>
       </c>
@@ -29353,7 +29361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="458" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>48</v>
       </c>
@@ -29418,7 +29426,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="459" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>48</v>
       </c>
@@ -29545,7 +29553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="461" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>24</v>
       </c>
@@ -29660,7 +29668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="463" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>48</v>
       </c>
@@ -29787,7 +29795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="465" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>48</v>
       </c>
@@ -29914,7 +29922,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="467" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>48</v>
       </c>
@@ -29988,7 +29996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="468" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>48</v>
       </c>
@@ -30062,7 +30070,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="469" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>24</v>
       </c>
@@ -30177,7 +30185,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="471" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>48</v>
       </c>
@@ -30239,7 +30247,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="472" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>48</v>
       </c>
@@ -30301,7 +30309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="473" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>48</v>
       </c>
@@ -30360,7 +30368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="474" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>48</v>
       </c>
@@ -30422,7 +30430,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="475" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>48</v>
       </c>
@@ -30484,7 +30492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="476" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>48</v>
       </c>
@@ -30543,7 +30551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="477" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>24</v>
       </c>
@@ -30608,7 +30616,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="478" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>24</v>
       </c>
@@ -30673,7 +30681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="479" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>146</v>
       </c>
@@ -30726,7 +30734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="480" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>146</v>
       </c>
@@ -30782,7 +30790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="481" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>146</v>
       </c>
@@ -30844,7 +30852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="482" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>146</v>
       </c>
@@ -30900,7 +30908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="483" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>146</v>
       </c>
@@ -30962,7 +30970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="484" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>146</v>
       </c>
@@ -31027,7 +31035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="485" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>146</v>
       </c>
@@ -31092,7 +31100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="486" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>146</v>
       </c>
@@ -31148,7 +31156,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="487" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>146</v>
       </c>
@@ -31207,7 +31215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="488" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>146</v>
       </c>
@@ -31269,7 +31277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="489" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>146</v>
       </c>
@@ -31328,7 +31336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="490" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>146</v>
       </c>
@@ -31384,7 +31392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="491" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>146</v>
       </c>
@@ -31440,7 +31448,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="492" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>24</v>
       </c>
@@ -31499,7 +31507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="493" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>48</v>
       </c>
@@ -31564,7 +31572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="494" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>48</v>
       </c>
@@ -31632,7 +31640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="495" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>48</v>
       </c>
@@ -31700,7 +31708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="496" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>48</v>
       </c>
@@ -31768,7 +31776,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="497" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>24</v>
       </c>
@@ -31827,7 +31835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="498" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>48</v>
       </c>
@@ -31895,7 +31903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="499" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>48</v>
       </c>
@@ -31963,7 +31971,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="500" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>48</v>
       </c>
@@ -32031,7 +32039,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="501" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>48</v>
       </c>
@@ -32105,7 +32113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="502" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>24</v>
       </c>
@@ -32164,7 +32172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="503" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>48</v>
       </c>
@@ -32223,7 +32231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="504" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>48</v>
       </c>
@@ -32288,7 +32296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="505" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>48</v>
       </c>
@@ -32347,7 +32355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="506" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>48</v>
       </c>
@@ -32409,7 +32417,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="507" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>48</v>
       </c>
@@ -32468,7 +32476,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="508" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>48</v>
       </c>
@@ -32530,7 +32538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="509" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>48</v>
       </c>
@@ -32595,7 +32603,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="510" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>48</v>
       </c>
@@ -32657,7 +32665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="511" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
         <v>48</v>
       </c>
@@ -32719,7 +32727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="512" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
         <v>48</v>
       </c>
@@ -32781,7 +32789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="513" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>48</v>
       </c>
@@ -32843,7 +32851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="514" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>48</v>
       </c>
@@ -32911,7 +32919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="515" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>48</v>
       </c>
@@ -32973,7 +32981,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="516" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>48</v>
       </c>
@@ -33032,7 +33040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="517" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>48</v>
       </c>
@@ -33100,7 +33108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="518" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>48</v>
       </c>
@@ -33168,7 +33176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="519" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>48</v>
       </c>
@@ -33230,7 +33238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="520" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>48</v>
       </c>
@@ -33295,7 +33303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="521" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521" t="s">
         <v>48</v>
       </c>
@@ -33360,7 +33368,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="522" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A522" t="s">
         <v>48</v>
       </c>
@@ -33428,7 +33436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="523" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>48</v>
       </c>
@@ -33496,7 +33504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="524" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>48</v>
       </c>
@@ -33561,7 +33569,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="525" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525" t="s">
         <v>48</v>
       </c>
@@ -33620,7 +33628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="526" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526" t="s">
         <v>48</v>
       </c>
@@ -33679,7 +33687,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="527" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A527" t="s">
         <v>48</v>
       </c>
@@ -33738,7 +33746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="528" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A528" t="s">
         <v>48</v>
       </c>
@@ -33797,7 +33805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="529" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A529" t="s">
         <v>48</v>
       </c>
@@ -33856,7 +33864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="530" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A530" t="s">
         <v>48</v>
       </c>
@@ -33915,7 +33923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="531" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A531" t="s">
         <v>48</v>
       </c>
@@ -33974,7 +33982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="532" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532" t="s">
         <v>48</v>
       </c>
@@ -34033,7 +34041,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="533" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533" t="s">
         <v>48</v>
       </c>
@@ -34092,7 +34100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="534" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534" t="s">
         <v>48</v>
       </c>
@@ -34151,7 +34159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="535" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535" t="s">
         <v>24</v>
       </c>
@@ -34210,7 +34218,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="536" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536" t="s">
         <v>48</v>
       </c>
@@ -34272,7 +34280,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="537" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537" t="s">
         <v>24</v>
       </c>
@@ -34331,7 +34339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="538" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A538" t="s">
         <v>48</v>
       </c>
@@ -34393,7 +34401,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="539" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A539" t="s">
         <v>48</v>
       </c>
@@ -34455,7 +34463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="540" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A540" t="s">
         <v>48</v>
       </c>
@@ -34517,7 +34525,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="541" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A541" t="s">
         <v>48</v>
       </c>
@@ -34576,7 +34584,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="542" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A542" t="s">
         <v>48</v>
       </c>
@@ -34638,7 +34646,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="543" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A543" t="s">
         <v>24</v>
       </c>
@@ -34697,7 +34705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="544" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544" t="s">
         <v>48</v>
       </c>
@@ -34821,7 +34829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="546" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A546" t="s">
         <v>48</v>
       </c>
@@ -34895,7 +34903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="547" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547" t="s">
         <v>24</v>
       </c>
@@ -34954,7 +34962,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="548" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548" t="s">
         <v>48</v>
       </c>
@@ -35016,7 +35024,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="549" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A549" t="s">
         <v>48</v>
       </c>
@@ -35078,7 +35086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="550" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550" t="s">
         <v>48</v>
       </c>
@@ -35137,7 +35145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="551" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="551" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A551" t="s">
         <v>48</v>
       </c>
@@ -35199,7 +35207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="552" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="552" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A552" t="s">
         <v>48</v>
       </c>
@@ -35261,7 +35269,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="553" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="553" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A553" t="s">
         <v>48</v>
       </c>
@@ -35320,7 +35328,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="554" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
         <v>48</v>
       </c>
@@ -35382,7 +35390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="555" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
         <v>48</v>
       </c>
@@ -35444,7 +35452,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="556" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
         <v>48</v>
       </c>
@@ -35506,7 +35514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="557" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
         <v>48</v>
       </c>
@@ -35568,7 +35576,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="558" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
         <v>48</v>
       </c>
@@ -35627,7 +35635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="559" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
         <v>48</v>
       </c>
@@ -35689,7 +35697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="560" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
         <v>48</v>
       </c>
@@ -35748,7 +35756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="561" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
         <v>258</v>
       </c>
@@ -35804,7 +35812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="562" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="562" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
         <v>258</v>
       </c>
@@ -35860,7 +35868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="563" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
         <v>258</v>
       </c>
@@ -35916,7 +35924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="564" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
         <v>258</v>
       </c>
@@ -35972,7 +35980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="565" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
         <v>258</v>
       </c>
@@ -36028,7 +36036,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="566" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
         <v>258</v>
       </c>
@@ -36087,7 +36095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="567" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
         <v>258</v>
       </c>
@@ -36146,7 +36154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="568" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
         <v>258</v>
       </c>
@@ -36202,7 +36210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="569" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
         <v>258</v>
       </c>
@@ -36261,7 +36269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="570" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
         <v>258</v>
       </c>
@@ -36317,7 +36325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="571" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
         <v>258</v>
       </c>
@@ -36373,7 +36381,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="572" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
         <v>258</v>
       </c>
@@ -36429,7 +36437,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="573" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
         <v>258</v>
       </c>
@@ -36482,7 +36490,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="574" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
         <v>146</v>
       </c>
@@ -36538,7 +36546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="575" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
         <v>146</v>
       </c>
@@ -36609,7 +36617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="576" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
         <v>146</v>
       </c>
@@ -36668,7 +36676,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="577" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
         <v>146</v>
       </c>
@@ -36724,7 +36732,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="578" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
         <v>146</v>
       </c>
@@ -36792,7 +36800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="579" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
         <v>146</v>
       </c>
@@ -36863,7 +36871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="580" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
         <v>146</v>
       </c>
@@ -36934,7 +36942,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="581" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
         <v>146</v>
       </c>
@@ -36990,7 +36998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="582" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
         <v>146</v>
       </c>
@@ -37049,7 +37057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="583" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
         <v>146</v>
       </c>
@@ -37114,7 +37122,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="584" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
         <v>146</v>
       </c>
@@ -37170,7 +37178,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="585" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
         <v>146</v>
       </c>
@@ -37226,7 +37234,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="586" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A586" t="s">
         <v>146</v>
       </c>
@@ -37298,7 +37306,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X586" xr:uid="{E5FDCEE0-F19C-462F-9C6A-117F5A0AAFD7}"/>
+  <autoFilter ref="A1:X586" xr:uid="{E5FDCEE0-F19C-462F-9C6A-117F5A0AAFD7}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Place 1 Ad for 30 days"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>